<commit_message>
Changes in POM and added classes to read data from excel and used data provider
</commit_message>
<xml_diff>
--- a/src/test/data/testBranchAddress.xlsx
+++ b/src/test/data/testBranchAddress.xlsx
@@ -46,11 +46,11 @@
 103 B Abhijeet 1, 1st Floor, Mithakali Six Roads, Ahmedabad 380 006.</t>
   </si>
   <si>
+    <t>Bangalore</t>
+  </si>
+  <si>
     <t>Mercury Travels Ltd.
 125, Infantry Road, Bangalore 560 001.</t>
-  </si>
-  <si>
-    <t>Bangalore</t>
   </si>
 </sst>
 </file>
@@ -389,7 +389,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -424,10 +424,10 @@
     </row>
     <row r="4" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Latest update on 7 September
</commit_message>
<xml_diff>
--- a/src/test/data/testBranchAddress.xlsx
+++ b/src/test/data/testBranchAddress.xlsx
@@ -38,19 +38,19 @@
     <t>Ahmedabad</t>
   </si>
   <si>
+    <t>Bangalore</t>
+  </si>
+  <si>
+    <t>Mercury Travels Ltd.
+125, Infantry Road, Bangalore 560 001.</t>
+  </si>
+  <si>
+    <t>Mercury Travels Ltd.
+103 B Abhijeet 1, 1st Floor, Mithakali Six Roads, Ahmedabad 380 006.</t>
+  </si>
+  <si>
     <t>Mercury Travels Ltd.
 C/o Hotel Clarks Shiraz, 54, Taj Road, Agra 282 001.</t>
-  </si>
-  <si>
-    <t>Mercury Travels Ltd.
-103 B Abhijeet 1, 1st Floor, Mithakali Six Roads, Ahmedabad 380 006.</t>
-  </si>
-  <si>
-    <t>Bangalore</t>
-  </si>
-  <si>
-    <t>Mercury Travels Ltd.
-125, Infantry Road, Bangalore 560 001.</t>
   </si>
 </sst>
 </file>
@@ -389,7 +389,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -411,7 +411,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -419,15 +419,15 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Latest Update on 15 Sep - Improved code for Extent report and attached screenshots when test fails
</commit_message>
<xml_diff>
--- a/src/test/data/testBranchAddress.xlsx
+++ b/src/test/data/testBranchAddress.xlsx
@@ -42,15 +42,15 @@
   </si>
   <si>
     <t>Mercury Travels Ltd.
-125, Infantry Road, Bangalore 560 001.</t>
+103 B Abhijeet 1, 1st Floor, Mithakali Six Roads, Ahmedabad 380 006.</t>
   </si>
   <si>
     <t>Mercury Travels Ltd.
-103 B Abhijeet 1, 1st Floor, Mithakali Six Roads, Ahmedabad 380 006.</t>
+125, Infantry Road, Bangalore 560 001xxx.</t>
   </si>
   <si>
     <t>Mercury Travels Ltd.
-C/o Hotel Clarks Shiraz, 54, Taj Road, Agra 282 001xx.</t>
+C/o Hotel Clarks Shiraz, 54, Taj Road, Agra 282 001.</t>
   </si>
 </sst>
 </file>
@@ -389,7 +389,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -419,7 +419,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -427,7 +427,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Latest update on 30th September
</commit_message>
<xml_diff>
--- a/src/test/data/testBranchAddress.xlsx
+++ b/src/test/data/testBranchAddress.xlsx
@@ -46,11 +46,11 @@
   </si>
   <si>
     <t>Mercury Travels Ltd.
-125, Infantry Road, Bangalore 560 001xxx.</t>
+C/o Hotel Clarks Shiraz, 54, Taj Road, Agra 282 001.</t>
   </si>
   <si>
     <t>Mercury Travels Ltd.
-C/o Hotel Clarks Shiraz, 54, Taj Road, Agra 282 001.</t>
+125, Infantry Road, Bangalore 560 001.</t>
   </si>
 </sst>
 </file>
@@ -389,7 +389,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -411,7 +411,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -427,7 +427,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>